<commit_message>
Add competition matching logic with ID_Name format and Telegram notifications
</commit_message>
<xml_diff>
--- a/competitions/Competitions_Results_Odds_Stake.xlsx
+++ b/competitions/Competitions_Results_Odds_Stake.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UpWork\Andrea Natali\BetfairItalyBot\competitions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BE1D59-8DD3-4AA2-9B39-C03F86F6FE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1" calcId="124519"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67" count="67">
-  <si>
-    <t>Campionato</t>
-  </si>
-  <si>
-    <t>Risultato</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="73">
   <si>
     <t>Under_%</t>
   </si>
@@ -28,18 +28,12 @@
     <t>Partite</t>
   </si>
   <si>
-    <t>Quota_Min_Back_Under</t>
-  </si>
-  <si>
     <t>Quota_Max_Lay_Over</t>
   </si>
   <si>
     <t>Affidabilità</t>
   </si>
   <si>
-    <t>Livello</t>
-  </si>
-  <si>
     <t>Argentina-Primera Division</t>
   </si>
   <si>
@@ -215,25 +209,57 @@
   </si>
   <si>
     <t>Competition</t>
+  </si>
+  <si>
+    <t>Competition-Live</t>
+  </si>
+  <si>
+    <t>Competition-Betfair</t>
+  </si>
+  <si>
+    <t>4_Serie A</t>
+  </si>
+  <si>
+    <t>81_Italian Serie A</t>
+  </si>
+  <si>
+    <t>2_Premier League</t>
+  </si>
+  <si>
+    <t>10932509_English Premier League</t>
+  </si>
+  <si>
+    <t>3_LaLiga Santander</t>
+  </si>
+  <si>
+    <t>117_Spanish La Liga</t>
+  </si>
+  <si>
+    <t>24_Serie A</t>
+  </si>
+  <si>
+    <t>13_Brazilian Serie A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -273,19 +299,30 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16" count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -332,7 +369,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,9 +401,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -398,6 +453,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -506,7 +579,7 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
@@ -573,87 +646,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="113">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="113" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" defaultColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="1" width="25.097656" style="0"/>
-    <col min="3" max="3" hidden="1" customWidth="1" bestFit="1" width="10.0" style="0"/>
-    <col min="4" max="4" hidden="1" customWidth="1" bestFit="1" width="10.0" style="0"/>
-    <col min="5" max="5" customWidth="1" width="21.597656" style="0"/>
-    <col min="6" max="6" hidden="1" customWidth="1" bestFit="1" width="10.0" style="0"/>
-    <col min="7" max="7" hidden="1" customWidth="1" bestFit="1" width="10.0" style="0"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="4" width="10" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1"/>
+    <col min="6" max="7" width="10" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="20.88671875" customWidth="1"/>
+    <col min="10" max="10" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="8:8" ht="15.55">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="8:8">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C2">
         <v>62.58</v>
       </c>
       <c r="D2">
-        <v>302.0</v>
+        <v>302</v>
       </c>
       <c r="E2">
         <v>1.67</v>
       </c>
       <c r="F2">
-        <v>1.529</v>
+        <v>1.5289999999999999</v>
       </c>
       <c r="G2">
-        <v>72.93819106455545</v>
+        <v>72.938191064555454</v>
       </c>
       <c r="H2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="3" spans="8:8" ht="15.05">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C3">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="E3">
         <v>1.75</v>
@@ -662,24 +743,24 @@
         <v>1.595</v>
       </c>
       <c r="G3">
-        <v>62.88761973629261</v>
+        <v>62.887619736292613</v>
       </c>
       <c r="H3">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4" spans="8:8" ht="15.05">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="D4">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>1.4</v>
@@ -688,76 +769,88 @@
         <v>1.276</v>
       </c>
       <c r="G4">
-        <v>69.49950251727819</v>
+        <v>69.499502517278188</v>
       </c>
       <c r="H4">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="5" spans="8:8" ht="15.05">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>65.52</v>
       </c>
       <c r="D5">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="E5">
         <v>1.6</v>
       </c>
       <c r="F5">
-        <v>1.461</v>
+        <v>1.4610000000000001</v>
       </c>
       <c r="G5">
-        <v>63.04252363607348</v>
+        <v>63.042523636073483</v>
       </c>
       <c r="H5">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6" spans="8:8" ht="15.05">
+        <v>2</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>62.5</v>
       </c>
       <c r="D6">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="E6">
         <v>1.68</v>
       </c>
       <c r="F6">
-        <v>1.531</v>
+        <v>1.5309999999999999</v>
       </c>
       <c r="G6">
-        <v>61.43072338416216</v>
+        <v>61.430723384162157</v>
       </c>
       <c r="H6">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" spans="8:8" ht="15.05">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C7">
-        <v>71.43</v>
+        <v>71.430000000000007</v>
       </c>
       <c r="D7">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="E7">
         <v>1.47</v>
@@ -766,24 +859,24 @@
         <v>1.34</v>
       </c>
       <c r="G7">
-        <v>68.13888683633694</v>
+        <v>68.138886836336937</v>
       </c>
       <c r="H7">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="8" spans="8:8" ht="15.05">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>60.61</v>
       </c>
       <c r="D8">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="E8">
         <v>1.73</v>
@@ -792,102 +885,102 @@
         <v>1.579</v>
       </c>
       <c r="G8">
-        <v>60.26470741301422</v>
+        <v>60.264707413014222</v>
       </c>
       <c r="H8">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9" spans="8:8" ht="15.05">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C9">
         <v>62.26</v>
       </c>
       <c r="D9">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="E9">
         <v>1.68</v>
       </c>
       <c r="F9">
-        <v>1.537</v>
+        <v>1.5369999999999999</v>
       </c>
       <c r="G9">
         <v>63.83675542472325</v>
       </c>
       <c r="H9">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="10" spans="8:8" ht="15.05">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C10">
-        <v>65.85</v>
+        <v>65.849999999999994</v>
       </c>
       <c r="D10">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="E10">
         <v>1.59</v>
       </c>
       <c r="F10">
-        <v>1.453</v>
+        <v>1.4530000000000001</v>
       </c>
       <c r="G10">
-        <v>65.04007900198314</v>
+        <v>65.040079001983145</v>
       </c>
       <c r="H10">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="11" spans="8:8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <v>61.46</v>
       </c>
       <c r="D11">
-        <v>192.0</v>
+        <v>192</v>
       </c>
       <c r="E11">
         <v>1.7</v>
       </c>
       <c r="F11">
-        <v>1.557</v>
+        <v>1.5569999999999999</v>
       </c>
       <c r="G11">
-        <v>69.84352477089872</v>
+        <v>69.843524770898725</v>
       </c>
       <c r="H11">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="12" spans="8:8" ht="15.05">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C12">
         <v>60.53</v>
       </c>
       <c r="D12">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>1.73</v>
@@ -896,24 +989,24 @@
         <v>1.581</v>
       </c>
       <c r="G12">
-        <v>60.92843094106598</v>
+        <v>60.928430941065983</v>
       </c>
       <c r="H12">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="13" spans="8:8" ht="15.05">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>63.89</v>
       </c>
       <c r="D13">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="E13">
         <v>1.64</v>
@@ -922,50 +1015,50 @@
         <v>1.498</v>
       </c>
       <c r="G13">
-        <v>63.00460277347313</v>
+        <v>63.004602773473131</v>
       </c>
       <c r="H13">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="14" spans="8:8" ht="15.05">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C14">
         <v>66.67</v>
       </c>
       <c r="D14">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="E14">
         <v>1.57</v>
       </c>
       <c r="F14">
-        <v>1.435</v>
+        <v>1.4350000000000001</v>
       </c>
       <c r="G14">
-        <v>63.4829701297124</v>
+        <v>63.482970129712399</v>
       </c>
       <c r="H14">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="15" spans="8:8" ht="15.05">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15">
-        <v>69.01</v>
+        <v>69.010000000000005</v>
       </c>
       <c r="D15">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="E15">
         <v>1.52</v>
@@ -974,50 +1067,50 @@
         <v>1.387</v>
       </c>
       <c r="G15">
-        <v>70.05339554050207</v>
+        <v>70.053395540502066</v>
       </c>
       <c r="H15">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="16" spans="8:8" ht="15.05">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>66.67</v>
       </c>
       <c r="D16">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="E16">
         <v>1.57</v>
       </c>
       <c r="F16">
-        <v>1.435</v>
+        <v>1.4350000000000001</v>
       </c>
       <c r="G16">
-        <v>64.50670741301421</v>
+        <v>64.506707413014212</v>
       </c>
       <c r="H16">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="17" spans="8:8" ht="15.05">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C17">
         <v>63.64</v>
       </c>
       <c r="D17">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="E17">
         <v>1.65</v>
@@ -1026,24 +1119,24 @@
         <v>1.504</v>
       </c>
       <c r="G17">
-        <v>68.52786905266612</v>
+        <v>68.527869052666119</v>
       </c>
       <c r="H17">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="18" spans="8:8" ht="15.05">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18">
         <v>60</v>
       </c>
-      <c r="C18">
-        <v>60.0</v>
-      </c>
       <c r="D18">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="E18">
         <v>1.75</v>
@@ -1052,50 +1145,50 @@
         <v>1.595</v>
       </c>
       <c r="G18">
-        <v>58.42134734544723</v>
+        <v>58.421347345447231</v>
       </c>
       <c r="H18">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19" spans="8:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C19">
-        <v>64.1</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="D19">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="E19">
         <v>1.63</v>
       </c>
       <c r="F19">
-        <v>1.493</v>
+        <v>1.4930000000000001</v>
       </c>
       <c r="G19">
-        <v>63.55994692114805</v>
+        <v>63.559946921148047</v>
       </c>
       <c r="H19">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="20" spans="8:8" ht="15.05">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C20">
         <v>60.61</v>
       </c>
       <c r="D20">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="E20">
         <v>1.73</v>
@@ -1104,76 +1197,76 @@
         <v>1.579</v>
       </c>
       <c r="G20">
-        <v>65.86936412291834</v>
+        <v>65.869364122918341</v>
       </c>
       <c r="H20">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="21" spans="8:8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C21">
         <v>61.11</v>
       </c>
       <c r="D21">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="E21">
         <v>1.71</v>
       </c>
       <c r="F21">
-        <v>1.566</v>
+        <v>1.5660000000000001</v>
       </c>
       <c r="G21">
-        <v>57.5224580966407</v>
+        <v>57.522458096640698</v>
       </c>
       <c r="H21">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="22" spans="8:8" ht="15.05">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C22">
         <v>63.49</v>
       </c>
       <c r="D22">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="E22">
         <v>1.65</v>
       </c>
       <c r="F22">
-        <v>1.507</v>
+        <v>1.5069999999999999</v>
       </c>
       <c r="G22">
-        <v>65.5795265834216</v>
+        <v>65.579526583421597</v>
       </c>
       <c r="H22">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="23" spans="8:8" ht="15.05">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C23">
         <v>61.36</v>
       </c>
       <c r="D23">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="E23">
         <v>1.71</v>
@@ -1182,50 +1275,50 @@
         <v>1.56</v>
       </c>
       <c r="G23">
-        <v>62.25734005677494</v>
+        <v>62.257340056774943</v>
       </c>
       <c r="H23">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="24" spans="8:8" ht="15.05">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C24">
         <v>61.45</v>
       </c>
       <c r="D24">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="E24">
         <v>1.71</v>
       </c>
       <c r="F24">
-        <v>1.557</v>
+        <v>1.5569999999999999</v>
       </c>
       <c r="G24">
-        <v>65.55806174975427</v>
+        <v>65.558061749754273</v>
       </c>
       <c r="H24">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="25" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C25">
         <v>63.89</v>
       </c>
       <c r="D25">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="E25">
         <v>1.64</v>
@@ -1234,76 +1327,76 @@
         <v>1.498</v>
       </c>
       <c r="G25">
-        <v>63.00460277347313</v>
+        <v>63.004602773473131</v>
       </c>
       <c r="H25">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="26" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C26">
-        <v>64.71</v>
+        <v>64.709999999999994</v>
       </c>
       <c r="D26">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="E26">
         <v>1.62</v>
       </c>
       <c r="F26">
-        <v>1.479</v>
+        <v>1.4790000000000001</v>
       </c>
       <c r="G26">
-        <v>65.35551667774187</v>
+        <v>65.355516677741875</v>
       </c>
       <c r="H26">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="27" spans="8:8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C27">
         <v>61.11</v>
       </c>
       <c r="D27">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="E27">
         <v>1.71</v>
       </c>
       <c r="F27">
-        <v>1.566</v>
+        <v>1.5660000000000001</v>
       </c>
       <c r="G27">
-        <v>64.59474745030556</v>
+        <v>64.594747450305562</v>
       </c>
       <c r="H27">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="28" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C28">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D28">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="E28">
         <v>1.75</v>
@@ -1312,76 +1405,76 @@
         <v>1.595</v>
       </c>
       <c r="G28">
-        <v>58.42134734544723</v>
+        <v>58.421347345447231</v>
       </c>
       <c r="H28">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="29" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C29">
         <v>62.65</v>
       </c>
       <c r="D29">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="E29">
         <v>1.67</v>
       </c>
       <c r="F29">
-        <v>1.527</v>
+        <v>1.5269999999999999</v>
       </c>
       <c r="G29">
-        <v>66.39806174975428</v>
+        <v>66.398061749754277</v>
       </c>
       <c r="H29">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="30" spans="8:8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C30">
         <v>61.11</v>
       </c>
       <c r="D30">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="E30">
         <v>1.71</v>
       </c>
       <c r="F30">
-        <v>1.566</v>
+        <v>1.5660000000000001</v>
       </c>
       <c r="G30">
-        <v>61.05860277347313</v>
+        <v>61.058602773473133</v>
       </c>
       <c r="H30">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="31" spans="8:8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C31">
         <v>62.96</v>
       </c>
       <c r="D31">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="E31">
         <v>1.66</v>
@@ -1390,76 +1483,82 @@
         <v>1.52</v>
       </c>
       <c r="G31">
-        <v>60.8859701297124</v>
+        <v>60.885970129712398</v>
       </c>
       <c r="H31">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="32" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C32">
         <v>62.16</v>
       </c>
       <c r="D32">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="E32">
         <v>1.68</v>
       </c>
       <c r="F32">
-        <v>1.539</v>
+        <v>1.5389999999999999</v>
       </c>
       <c r="G32">
-        <v>61.9333807880756</v>
+        <v>61.933380788075603</v>
       </c>
       <c r="H32">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="33" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C33">
         <v>60.87</v>
       </c>
       <c r="D33">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="E33">
         <v>1.72</v>
       </c>
       <c r="F33">
-        <v>1.572</v>
+        <v>1.5720000000000001</v>
       </c>
       <c r="G33">
-        <v>62.14111420806513</v>
+        <v>62.141114208065133</v>
       </c>
       <c r="H33">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="34" spans="8:8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C34">
         <v>67.86</v>
       </c>
       <c r="D34">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="E34">
         <v>1.54</v>
@@ -1468,76 +1567,76 @@
         <v>1.41</v>
       </c>
       <c r="G34">
-        <v>64.50150251727818</v>
+        <v>64.501502517278183</v>
       </c>
       <c r="H34">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="35" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C35">
-        <v>64.71</v>
+        <v>64.709999999999994</v>
       </c>
       <c r="D35">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="E35">
         <v>1.61</v>
       </c>
       <c r="F35">
-        <v>1.479</v>
+        <v>1.4790000000000001</v>
       </c>
       <c r="G35">
-        <v>63.28700464467018</v>
+        <v>63.287004644670183</v>
       </c>
       <c r="H35">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="36" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C36">
         <v>61.61</v>
       </c>
       <c r="D36">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="E36">
         <v>1.7</v>
       </c>
       <c r="F36">
-        <v>1.553</v>
+        <v>1.5529999999999999</v>
       </c>
       <c r="G36">
         <v>67.19879187094304</v>
       </c>
       <c r="H36">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="37" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37">
+        <v>68</v>
+      </c>
+      <c r="D37">
         <v>25</v>
-      </c>
-      <c r="B37" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37">
-        <v>68.0</v>
-      </c>
-      <c r="D37">
-        <v>25.0</v>
       </c>
       <c r="E37">
         <v>1.54</v>
@@ -1546,50 +1645,50 @@
         <v>1.407</v>
       </c>
       <c r="G37">
-        <v>64.02134734544723</v>
+        <v>64.021347345447225</v>
       </c>
       <c r="H37">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="38" spans="8:8" ht="15.0" hidden="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C38">
         <v>62.5</v>
       </c>
       <c r="D38">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="E38">
-        <v>1.672</v>
+        <v>1.6719999999999999</v>
       </c>
       <c r="F38">
-        <v>1.531</v>
+        <v>1.5309999999999999</v>
       </c>
       <c r="G38">
-        <v>59.96309074040143</v>
+        <v>59.963090740401427</v>
       </c>
       <c r="H38">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="39" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C39">
-        <v>71.43</v>
+        <v>71.430000000000007</v>
       </c>
       <c r="D39">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="E39">
         <v>1.46</v>
@@ -1598,24 +1697,24 @@
         <v>1.34</v>
       </c>
       <c r="G39">
-        <v>67.00050251727819</v>
+        <v>67.000502517278193</v>
       </c>
       <c r="H39">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="40" spans="8:8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C40">
         <v>67.86</v>
       </c>
       <c r="D40">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="E40">
         <v>1.54</v>
@@ -1624,76 +1723,82 @@
         <v>1.41</v>
       </c>
       <c r="G40">
-        <v>64.50150251727818</v>
+        <v>64.501502517278183</v>
       </c>
       <c r="H40">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="41" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B41" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C41">
         <v>65.22</v>
       </c>
       <c r="D41">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="E41">
         <v>1.6</v>
       </c>
       <c r="F41">
-        <v>1.467</v>
+        <v>1.4670000000000001</v>
       </c>
       <c r="G41">
-        <v>65.18611420806513</v>
+        <v>65.186114208065135</v>
       </c>
       <c r="H41">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="42" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C42">
         <v>63.01</v>
       </c>
       <c r="D42">
-        <v>246.0</v>
+        <v>246</v>
       </c>
       <c r="E42">
         <v>1.66</v>
       </c>
       <c r="F42">
-        <v>1.519</v>
+        <v>1.5189999999999999</v>
       </c>
       <c r="G42">
-        <v>72.19288038871973</v>
+        <v>72.192880388719729</v>
       </c>
       <c r="H42">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="43" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B43" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C43">
         <v>63.04</v>
       </c>
       <c r="D43">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="E43">
         <v>1.66</v>
@@ -1702,50 +1807,50 @@
         <v>1.518</v>
       </c>
       <c r="G43">
-        <v>63.66011420806514</v>
+        <v>63.660114208065139</v>
       </c>
       <c r="H43">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="44" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C44">
         <v>65.06</v>
       </c>
       <c r="D44">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="E44">
         <v>1.61</v>
       </c>
       <c r="F44">
-        <v>1.471</v>
+        <v>1.4710000000000001</v>
       </c>
       <c r="G44">
-        <v>68.08506174975429</v>
+        <v>68.085061749754288</v>
       </c>
       <c r="H44">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="45" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C45">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D45">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="E45">
         <v>1.74</v>
@@ -1754,50 +1859,50 @@
         <v>1.595</v>
       </c>
       <c r="G45">
-        <v>61.95749202227967</v>
+        <v>61.957492022279673</v>
       </c>
       <c r="H45">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="46" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B46" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C46">
         <v>63.16</v>
       </c>
       <c r="D46">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="E46">
         <v>1.65</v>
       </c>
       <c r="F46">
-        <v>1.515</v>
+        <v>1.5149999999999999</v>
       </c>
       <c r="G46">
-        <v>62.76943094106599</v>
+        <v>62.769430941065991</v>
       </c>
       <c r="H46">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="47" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C47">
         <v>61.9</v>
       </c>
       <c r="D47">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="E47">
         <v>1.69</v>
@@ -1806,76 +1911,76 @@
         <v>1.546</v>
       </c>
       <c r="G47">
-        <v>62.39801455034988</v>
+        <v>62.398014550349878</v>
       </c>
       <c r="H47">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="48" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C48">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="D48">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="E48">
         <v>1.68</v>
       </c>
       <c r="F48">
-        <v>1.543</v>
+        <v>1.5429999999999999</v>
       </c>
       <c r="G48">
-        <v>63.35749202227966</v>
+        <v>63.357492022279658</v>
       </c>
       <c r="H48">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="49" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C49">
         <v>65.12</v>
       </c>
       <c r="D49">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="E49">
         <v>1.6</v>
       </c>
       <c r="F49">
-        <v>1.469</v>
+        <v>1.4690000000000001</v>
       </c>
       <c r="G49">
-        <v>64.77205722742326</v>
+        <v>64.772057227423261</v>
       </c>
       <c r="H49">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="50" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C50">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="D50">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="E50">
         <v>1.54</v>
@@ -1884,50 +1989,50 @@
         <v>1.407</v>
       </c>
       <c r="G50">
-        <v>64.02134734544723</v>
+        <v>64.021347345447225</v>
       </c>
       <c r="H50">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="51" spans="8:8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C51">
         <v>63.33</v>
       </c>
       <c r="D51">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="E51">
         <v>1.65</v>
       </c>
       <c r="F51">
-        <v>1.511</v>
+        <v>1.5109999999999999</v>
       </c>
       <c r="G51">
-        <v>61.68247505946017</v>
+        <v>61.682475059460167</v>
       </c>
       <c r="H51">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="52" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C52">
         <v>60.98</v>
       </c>
       <c r="D52">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="E52">
         <v>1.71</v>
@@ -1936,50 +2041,50 @@
         <v>1.569</v>
       </c>
       <c r="G52">
-        <v>61.63107900198315</v>
+        <v>61.631079001983153</v>
       </c>
       <c r="H52">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="53" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C53">
-        <v>65.79</v>
+        <v>65.790000000000006</v>
       </c>
       <c r="D53">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="E53">
         <v>1.59</v>
       </c>
       <c r="F53">
-        <v>1.455</v>
+        <v>1.4550000000000001</v>
       </c>
       <c r="G53">
-        <v>64.610430941066</v>
+        <v>64.610430941065999</v>
       </c>
       <c r="H53">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="54" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C54">
         <v>61.64</v>
       </c>
       <c r="D54">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="E54">
         <v>1.69</v>
@@ -1988,76 +2093,76 @@
         <v>1.552</v>
       </c>
       <c r="G54">
-        <v>65.03611516441022</v>
+        <v>65.036115164410219</v>
       </c>
       <c r="H54">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="55" spans="8:8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C55">
         <v>64.52</v>
       </c>
       <c r="D55">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="E55">
         <v>1.62</v>
       </c>
       <c r="F55">
-        <v>1.483</v>
+        <v>1.4830000000000001</v>
       </c>
       <c r="G55">
-        <v>62.68275491095741</v>
+        <v>62.682754910957406</v>
       </c>
       <c r="H55">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="56" spans="8:8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C56">
         <v>73.08</v>
       </c>
       <c r="D56">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="E56">
         <v>1.43</v>
       </c>
       <c r="F56">
-        <v>1.309</v>
+        <v>1.3089999999999999</v>
       </c>
       <c r="G56">
-        <v>67.77743488807636</v>
+        <v>67.777434888076357</v>
       </c>
       <c r="H56">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="57" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C57">
         <v>65.38</v>
       </c>
       <c r="D57">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="E57">
         <v>1.6</v>
@@ -2066,24 +2171,24 @@
         <v>1.464</v>
       </c>
       <c r="G57">
-        <v>62.38743488807635</v>
+        <v>62.387434888076349</v>
       </c>
       <c r="H57">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="58" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C58">
         <v>60.45</v>
       </c>
       <c r="D58">
-        <v>177.0</v>
+        <v>177</v>
       </c>
       <c r="E58">
         <v>1.73</v>
@@ -2092,24 +2197,24 @@
         <v>1.583</v>
       </c>
       <c r="G58">
-        <v>68.72153361461031</v>
+        <v>68.721533614610308</v>
       </c>
       <c r="H58">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="59" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C59">
         <v>65.63</v>
       </c>
       <c r="D59">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="E59">
         <v>1.59</v>
@@ -2118,24 +2223,24 @@
         <v>1.458</v>
       </c>
       <c r="G59">
-        <v>63.62172338416215</v>
+        <v>63.621723384162152</v>
       </c>
       <c r="H59">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="60" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C60">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D60">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="E60">
         <v>1.74</v>
@@ -2144,24 +2249,24 @@
         <v>1.595</v>
       </c>
       <c r="G60">
-        <v>62.4437243758337</v>
+        <v>62.443724375833703</v>
       </c>
       <c r="H60">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="61" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C61">
-        <v>64.15</v>
+        <v>64.150000000000006</v>
       </c>
       <c r="D61">
-        <v>106.0</v>
+        <v>106</v>
       </c>
       <c r="E61">
         <v>1.63</v>
@@ -2170,50 +2275,50 @@
         <v>1.492</v>
       </c>
       <c r="G61">
-        <v>68.6959001015557</v>
+        <v>68.695900101555694</v>
       </c>
       <c r="H61">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="62" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C62">
         <v>65.22</v>
       </c>
       <c r="D62">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="E62">
         <v>1.6</v>
       </c>
       <c r="F62">
-        <v>1.467</v>
+        <v>1.4670000000000001</v>
       </c>
       <c r="G62">
-        <v>61.6499695312327</v>
+        <v>61.649969531232699</v>
       </c>
       <c r="H62">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="63" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C63">
         <v>63.39</v>
       </c>
       <c r="D63">
-        <v>112.0</v>
+        <v>112</v>
       </c>
       <c r="E63">
         <v>1.65</v>
@@ -2225,47 +2330,47 @@
         <v>68.44479187094305</v>
       </c>
       <c r="H63">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="64" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B64" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C64">
         <v>61.54</v>
       </c>
       <c r="D64">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="E64">
         <v>1.7</v>
       </c>
       <c r="F64">
-        <v>1.555</v>
+        <v>1.5549999999999999</v>
       </c>
       <c r="G64">
-        <v>59.69943488807635</v>
+        <v>59.699434888076347</v>
       </c>
       <c r="H64">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="65" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C65">
-        <v>71.43</v>
+        <v>71.430000000000007</v>
       </c>
       <c r="D65">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="E65">
         <v>1.46</v>
@@ -2274,50 +2379,50 @@
         <v>1.34</v>
       </c>
       <c r="G65">
-        <v>67.00050251727819</v>
+        <v>67.000502517278193</v>
       </c>
       <c r="H65">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="66" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B66" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C66">
         <v>65.52</v>
       </c>
       <c r="D66">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="E66">
         <v>1.59</v>
       </c>
       <c r="F66">
-        <v>1.461</v>
+        <v>1.4610000000000001</v>
       </c>
       <c r="G66">
-        <v>63.04252363607348</v>
+        <v>63.042523636073483</v>
       </c>
       <c r="H66">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="67" spans="8:8" ht="15.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B67" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C67">
         <v>68.89</v>
       </c>
       <c r="D67">
-        <v>180.0</v>
+        <v>180</v>
       </c>
       <c r="E67">
         <v>1.52</v>
@@ -2326,50 +2431,50 @@
         <v>1.389</v>
       </c>
       <c r="G67">
-        <v>74.71527644619674</v>
+        <v>74.715276446196739</v>
       </c>
       <c r="H67">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="68" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B68" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C68">
         <v>63.83</v>
       </c>
       <c r="D68">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="E68">
         <v>1.64</v>
       </c>
       <c r="F68">
-        <v>1.499</v>
+        <v>1.4990000000000001</v>
       </c>
       <c r="G68">
-        <v>64.32282979985264</v>
+        <v>64.322829799852641</v>
       </c>
       <c r="H68">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="69" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B69" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C69">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="D69">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="E69">
         <v>1.39</v>
@@ -2378,50 +2483,50 @@
         <v>1.276</v>
       </c>
       <c r="G69">
-        <v>69.49950251727819</v>
+        <v>69.499502517278188</v>
       </c>
       <c r="H69">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="70" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B70" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C70">
         <v>62.16</v>
       </c>
       <c r="D70">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="E70">
         <v>1.68</v>
       </c>
       <c r="F70">
-        <v>1.539</v>
+        <v>1.5389999999999999</v>
       </c>
       <c r="G70">
-        <v>65.46952546490803</v>
+        <v>65.469525464908031</v>
       </c>
       <c r="H70">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="71" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B71" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C71">
         <v>63.86</v>
       </c>
       <c r="D71">
-        <v>83.0</v>
+        <v>83</v>
       </c>
       <c r="E71">
         <v>1.64</v>
@@ -2430,50 +2535,50 @@
         <v>1.498</v>
       </c>
       <c r="G71">
-        <v>67.24506174975429</v>
+        <v>67.245061749754285</v>
       </c>
       <c r="H71">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="72" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B72" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C72">
         <v>66.67</v>
       </c>
       <c r="D72">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="E72">
         <v>1.57</v>
       </c>
       <c r="F72">
-        <v>1.435</v>
+        <v>1.4350000000000001</v>
       </c>
       <c r="G72">
-        <v>64.02047505946018</v>
+        <v>64.020475059460182</v>
       </c>
       <c r="H72">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="73" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C73">
-        <v>64.76</v>
+        <v>64.760000000000005</v>
       </c>
       <c r="D73">
-        <v>105.0</v>
+        <v>105</v>
       </c>
       <c r="E73">
         <v>1.61</v>
@@ -2482,50 +2587,50 @@
         <v>1.478</v>
       </c>
       <c r="G73">
-        <v>69.07454354624107</v>
+        <v>69.074543546241074</v>
       </c>
       <c r="H73">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="74" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B74" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C74">
-        <v>68.57</v>
+        <v>68.569999999999993</v>
       </c>
       <c r="D74">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="E74">
         <v>1.52</v>
       </c>
       <c r="F74">
-        <v>1.396</v>
+        <v>1.3959999999999999</v>
       </c>
       <c r="G74">
-        <v>66.13688683633693</v>
+        <v>66.136886836336927</v>
       </c>
       <c r="H74">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="75" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B75" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C75">
         <v>62.3</v>
       </c>
       <c r="D75">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="E75">
         <v>1.68</v>
@@ -2534,24 +2639,30 @@
         <v>1.536</v>
       </c>
       <c r="G75">
-        <v>64.58194526591434</v>
+        <v>64.581945265914342</v>
       </c>
       <c r="H75">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="76" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B76" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C76">
         <v>60.61</v>
       </c>
       <c r="D76">
-        <v>358.0</v>
+        <v>358</v>
       </c>
       <c r="E76">
         <v>1.72</v>
@@ -2560,24 +2671,24 @@
         <v>1.579</v>
       </c>
       <c r="G76">
-        <v>72.42699999999999</v>
+        <v>72.426999999999992</v>
       </c>
       <c r="H76">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="77" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B77" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C77">
-        <v>64.29</v>
+        <v>64.290000000000006</v>
       </c>
       <c r="D77">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="E77">
         <v>1.62</v>
@@ -2586,76 +2697,76 @@
         <v>1.488</v>
       </c>
       <c r="G77">
-        <v>64.07101455034989</v>
+        <v>64.071014550349886</v>
       </c>
       <c r="H77">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="78" spans="8:8" ht="15.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B78" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C78">
         <v>62.03</v>
       </c>
       <c r="D78">
-        <v>79.0</v>
+        <v>79</v>
       </c>
       <c r="E78">
         <v>1.68</v>
       </c>
       <c r="F78">
-        <v>1.543</v>
+        <v>1.5429999999999999</v>
       </c>
       <c r="G78">
-        <v>65.71208073658522</v>
+        <v>65.712080736585222</v>
       </c>
       <c r="H78">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="79" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B79" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C79">
         <v>60.71</v>
       </c>
       <c r="D79">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="E79">
         <v>1.72</v>
       </c>
       <c r="F79">
-        <v>1.576</v>
+        <v>1.5760000000000001</v>
       </c>
       <c r="G79">
-        <v>59.49650251727819</v>
+        <v>59.496502517278188</v>
       </c>
       <c r="H79">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="80" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>45</v>
+      </c>
+      <c r="B80" t="s">
         <v>49</v>
       </c>
-      <c r="B80" t="s">
-        <v>53</v>
-      </c>
       <c r="C80">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D80">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="E80">
         <v>1.74</v>
@@ -2664,24 +2775,24 @@
         <v>1.595</v>
       </c>
       <c r="G80">
-        <v>60.81910770322091</v>
+        <v>60.819107703220908</v>
       </c>
       <c r="H80">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="81" spans="8:8" ht="15.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B81" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C81">
         <v>62.14</v>
       </c>
       <c r="D81">
-        <v>103.0</v>
+        <v>103</v>
       </c>
       <c r="E81">
         <v>1.68</v>
@@ -2690,50 +2801,50 @@
         <v>1.54</v>
       </c>
       <c r="G81">
-        <v>67.14243324583617</v>
+        <v>67.142433245836173</v>
       </c>
       <c r="H81">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="82" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B82" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C82">
         <v>69.23</v>
       </c>
       <c r="D82">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="E82">
         <v>1.51</v>
       </c>
       <c r="F82">
-        <v>1.382</v>
+        <v>1.3819999999999999</v>
       </c>
       <c r="G82">
-        <v>65.08243488807636</v>
+        <v>65.082434888076364</v>
       </c>
       <c r="H82">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="83" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C83">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="D83">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="E83">
         <v>1.74</v>
@@ -2742,24 +2853,24 @@
         <v>1.595</v>
       </c>
       <c r="G83">
-        <v>65.97986905266612</v>
+        <v>65.979869052666118</v>
       </c>
       <c r="H83">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="84" spans="8:8" ht="15.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84" t="s">
         <v>51</v>
-      </c>
-      <c r="B84" t="s">
-        <v>55</v>
       </c>
       <c r="C84">
         <v>76.92</v>
       </c>
       <c r="D84">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="E84">
         <v>1.36</v>
@@ -2768,24 +2879,24 @@
         <v>1.244</v>
       </c>
       <c r="G84">
-        <v>70.46543488807636</v>
+        <v>70.465434888076359</v>
       </c>
       <c r="H84">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="85" spans="8:8" ht="15.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B85" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C85">
         <v>63.64</v>
       </c>
       <c r="D85">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="E85">
         <v>1.64</v>
@@ -2794,39 +2905,40 @@
         <v>1.504</v>
       </c>
       <c r="G85">
-        <v>60.3171953799425</v>
+        <v>60.317195379942497</v>
       </c>
       <c r="H85">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="86" spans="8:8" ht="15.55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B86" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C86">
         <v>61.43</v>
       </c>
       <c r="D86">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="E86">
         <v>1.7</v>
       </c>
       <c r="F86">
-        <v>1.558</v>
+        <v>1.5580000000000001</v>
       </c>
       <c r="G86">
-        <v>64.67503151316937</v>
+        <v>64.675031513169372</v>
       </c>
       <c r="H86">
-        <v>3.0</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel files: Competitions_Results_Odds_Stake.xlsx and remove TEST file
</commit_message>
<xml_diff>
--- a/competitions/Competitions_Results_Odds_Stake.xlsx
+++ b/competitions/Competitions_Results_Odds_Stake.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\UpWork\Andrea Natali\BetfairItalyBot\competitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A4DF07-9536-4484-BDB5-9467CED9DA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7EF35E-465B-4433-AA8D-97A069D2D0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="144" yWindow="720" windowWidth="22896" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="144" yWindow="0" windowWidth="22896" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="73">
   <si>
     <t>Under_%</t>
   </si>
@@ -648,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J87"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="113" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -660,7 +660,8 @@
     <col min="3" max="4" width="10" hidden="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.77734375" customWidth="1"/>
     <col min="6" max="7" width="10" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="17.44140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="22.21875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -2779,7 +2780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>46</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>46</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>47</v>
       </c>
@@ -2857,7 +2858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>47</v>
       </c>
@@ -2883,7 +2884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>47</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>48</v>
       </c>
@@ -2935,15 +2936,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I87" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor: Consolidate code into services directory and improve logging
</commit_message>
<xml_diff>
--- a/competitions/Competitions_Results_Odds_Stake.xlsx
+++ b/competitions/Competitions_Results_Odds_Stake.xlsx
@@ -116,6 +116,7 @@
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Bulgarian A League</t>
     </r>
@@ -151,7 +152,7 @@
     <t xml:space="preserve">17_1.HNL</t>
   </si>
   <si>
-    <t xml:space="preserve">17_Croatian 1 HNL</t>
+    <t xml:space="preserve">17_Croatian HNL</t>
   </si>
   <si>
     <t xml:space="preserve">3-0</t>
@@ -190,7 +191,7 @@
     <t xml:space="preserve">77_Championship</t>
   </si>
   <si>
-    <t xml:space="preserve">7129730_English Championship</t>
+    <t xml:space="preserve">7129730_English Sky Bet Championship</t>
   </si>
   <si>
     <t xml:space="preserve">0-2</t>
@@ -202,7 +203,7 @@
     <t xml:space="preserve">82_League 1</t>
   </si>
   <si>
-    <t xml:space="preserve">35_English League 1</t>
+    <t xml:space="preserve">35_English Sky Bet League 1</t>
   </si>
   <si>
     <t xml:space="preserve">England-League Two</t>
@@ -211,7 +212,7 @@
     <t xml:space="preserve">83_League 2</t>
   </si>
   <si>
-    <t xml:space="preserve">37_English League 2</t>
+    <t xml:space="preserve">37_English Sky Bet League 2</t>
   </si>
   <si>
     <t xml:space="preserve">1-3</t>
@@ -401,6 +402,7 @@
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Scottish Premiership</t>
     </r>
@@ -430,7 +432,7 @@
     <t xml:space="preserve">63_Super League</t>
   </si>
   <si>
-    <t xml:space="preserve">113_Slovakian Super Liga</t>
+    <t xml:space="preserve">12013300_Slovakian Super Liga</t>
   </si>
   <si>
     <t xml:space="preserve">Slovenia-2. SNL</t>
@@ -491,6 +493,7 @@
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Swedish Allsvenskan</t>
     </r>
@@ -518,6 +521,7 @@
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Swiss Challenge League</t>
     </r>
@@ -538,7 +542,7 @@
     <t xml:space="preserve">76_Major League Soccer</t>
   </si>
   <si>
-    <t xml:space="preserve">141_US Major League Soccer</t>
+    <t xml:space="preserve">141_US MLS</t>
   </si>
   <si>
     <t xml:space="preserve">Wales-Premier League</t>
@@ -557,7 +561,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +596,19 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -643,29 +660,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -862,2736 +887,2744 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M87" activeCellId="0" sqref="M87"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J84" activeCellId="0" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="44.32"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>62.58</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>302</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>1.67</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>1.529</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>72.9381910645555</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>1.75</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>1.595</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>62.8876197362926</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>1.4</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>1.276</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>69.4995025172782</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>65.52</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>1.461</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>63.0425236360735</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>62.5</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>1.68</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>1.531</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>61.4307233841622</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="I6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="J6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>71.43</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>1.47</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>1.34</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>68.1388868363369</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="I7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="J7" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>60.61</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>1.73</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>1.579</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>60.2647074130142</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>62.26</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>53</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>1.68</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>1.537</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>63.8367554247233</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="J9" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>65.85</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>1.59</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>1.453</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>65.0400790019831</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="0" t="s">
+      <c r="J10" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>61.46</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>192</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>1.7</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>1.557</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>69.8435247708987</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>60.53</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>1.73</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>1.581</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>60.928430941066</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>63.89</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>1.64</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>1.498</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>63.0046027734731</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>66.67</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>1.57</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>1.435</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>63.4829701297124</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>69.01</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <v>71</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>1.52</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>1.387</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>70.0533955405021</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>66.67</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>1.57</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>1.435</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>64.5067074130142</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>63.64</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>1.65</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>1.504</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>68.5278690526661</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I17" s="0" t="s">
+      <c r="I17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J17" s="0" t="s">
+      <c r="J17" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>1.75</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>1.595</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>58.4213473454472</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I18" s="0" t="s">
+      <c r="I18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="0" t="s">
+      <c r="J18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>64.1</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>1.63</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>1.493</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>63.5599469211481</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I19" s="0" t="s">
+      <c r="I19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J19" s="0" t="s">
+      <c r="J19" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>60.61</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>1.73</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>1.579</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>65.8693641229183</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="I20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="J20" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>61.11</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>1.71</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>1.566</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>57.5224580966407</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>63.49</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>63</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>1.65</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>1.507</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <v>65.5795265834216</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I22" s="0" t="s">
+      <c r="I22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J22" s="0" t="s">
+      <c r="J22" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>61.36</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>44</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>1.71</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>1.56</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="1" t="n">
         <v>62.2573400567749</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="I23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J23" s="0" t="s">
+      <c r="J23" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>61.45</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>1.71</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>1.557</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>65.5580617497543</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="I24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="J24" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>63.89</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>1.64</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>1.498</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>63.0046027734731</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="I25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="J25" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>64.71</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>51</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>1.62</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>1.479</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="1" t="n">
         <v>65.3555166777419</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="I26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="J26" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>61.11</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>72</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>1.71</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>1.566</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>64.5947474503056</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="I27" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="J27" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>1.75</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="1" t="n">
         <v>1.595</v>
       </c>
-      <c r="G28" s="0" t="n">
+      <c r="G28" s="1" t="n">
         <v>58.4213473454472</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="I28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="J28" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>62.65</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>1.67</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="1" t="n">
         <v>1.527</v>
       </c>
-      <c r="G29" s="0" t="n">
+      <c r="G29" s="1" t="n">
         <v>66.3980617497543</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="I29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="J29" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <v>61.11</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>1.71</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="1" t="n">
         <v>1.566</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G30" s="1" t="n">
         <v>61.0586027734731</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="I30" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="J30" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="C31" s="1" t="n">
         <v>62.96</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>27</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>1.66</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="1" t="n">
         <v>1.52</v>
       </c>
-      <c r="G31" s="0" t="n">
+      <c r="G31" s="1" t="n">
         <v>60.8859701297124</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="I31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="C32" s="1" t="n">
         <v>62.16</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>37</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>1.68</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="1" t="n">
         <v>1.539</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G32" s="1" t="n">
         <v>61.9333807880756</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I32" s="0" t="s">
+      <c r="I32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J32" s="0" t="s">
+      <c r="J32" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="C33" s="1" t="n">
         <v>60.87</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>1.72</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="1" t="n">
         <v>1.572</v>
       </c>
-      <c r="G33" s="0" t="n">
+      <c r="G33" s="1" t="n">
         <v>62.1411142080651</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="I33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="J33" s="0" t="s">
+      <c r="J33" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="C34" s="1" t="n">
         <v>67.86</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>1.54</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="1" t="n">
         <v>1.41</v>
       </c>
-      <c r="G34" s="0" t="n">
+      <c r="G34" s="1" t="n">
         <v>64.5015025172782</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="I34" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J34" s="6" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="C35" s="1" t="n">
         <v>64.71</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="1" t="n">
         <v>34</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>1.61</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35" s="1" t="n">
         <v>1.479</v>
       </c>
-      <c r="G35" s="0" t="n">
+      <c r="G35" s="1" t="n">
         <v>63.2870046446702</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="I35" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="J35" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="C36" s="1" t="n">
         <v>61.61</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>1.7</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36" s="1" t="n">
         <v>1.553</v>
       </c>
-      <c r="G36" s="0" t="n">
+      <c r="G36" s="1" t="n">
         <v>67.198791870943</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I36" s="0" t="s">
+      <c r="I36" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="J36" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="C37" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="D37" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E37" s="0" t="n">
+      <c r="E37" s="1" t="n">
         <v>1.54</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="1" t="n">
         <v>1.407</v>
       </c>
-      <c r="G37" s="0" t="n">
+      <c r="G37" s="1" t="n">
         <v>64.0213473454472</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="H37" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I37" s="0" t="s">
+      <c r="I37" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J37" s="0" t="s">
+      <c r="J37" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="C38" s="1" t="n">
         <v>71.43</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="D38" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E38" s="0" t="n">
+      <c r="E38" s="1" t="n">
         <v>1.46</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38" s="1" t="n">
         <v>1.34</v>
       </c>
-      <c r="G38" s="0" t="n">
+      <c r="G38" s="1" t="n">
         <v>67.0005025172782</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H38" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I38" s="0" t="s">
+      <c r="I38" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J38" s="0" t="s">
+      <c r="J38" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="C39" s="1" t="n">
         <v>67.86</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="D39" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E39" s="0" t="n">
+      <c r="E39" s="1" t="n">
         <v>1.54</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F39" s="1" t="n">
         <v>1.41</v>
       </c>
-      <c r="G39" s="0" t="n">
+      <c r="G39" s="1" t="n">
         <v>64.5015025172782</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="H39" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="I39" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="J39" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="C40" s="1" t="n">
         <v>65.22</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="D40" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="E40" s="0" t="n">
+      <c r="E40" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="F40" s="1" t="n">
         <v>1.467</v>
       </c>
-      <c r="G40" s="0" t="n">
+      <c r="G40" s="1" t="n">
         <v>65.1861142080651</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="H40" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I40" s="0" t="s">
+      <c r="I40" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J40" s="0" t="s">
+      <c r="J40" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="C41" s="1" t="n">
         <v>63.01</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="D41" s="1" t="n">
         <v>246</v>
       </c>
-      <c r="E41" s="0" t="n">
+      <c r="E41" s="1" t="n">
         <v>1.66</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41" s="1" t="n">
         <v>1.519</v>
       </c>
-      <c r="G41" s="0" t="n">
+      <c r="G41" s="1" t="n">
         <v>72.1928803887197</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="H41" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I41" s="0" t="s">
+      <c r="I41" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J41" s="0" t="s">
+      <c r="J41" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="C42" s="1" t="n">
         <v>63.04</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="D42" s="1" t="n">
         <v>46</v>
       </c>
-      <c r="E42" s="0" t="n">
+      <c r="E42" s="1" t="n">
         <v>1.66</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42" s="1" t="n">
         <v>1.518</v>
       </c>
-      <c r="G42" s="0" t="n">
+      <c r="G42" s="1" t="n">
         <v>63.6601142080651</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I42" s="0" t="s">
+      <c r="I42" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J42" s="0" t="s">
+      <c r="J42" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="C43" s="1" t="n">
         <v>65.06</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="D43" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="E43" s="0" t="n">
+      <c r="E43" s="1" t="n">
         <v>1.61</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="F43" s="1" t="n">
         <v>1.471</v>
       </c>
-      <c r="G43" s="0" t="n">
+      <c r="G43" s="1" t="n">
         <v>68.0850617497543</v>
       </c>
-      <c r="H43" s="0" t="n">
+      <c r="H43" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I43" s="0" t="s">
+      <c r="I43" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J43" s="0" t="s">
+      <c r="J43" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="C44" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="D44" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="E44" s="0" t="n">
+      <c r="E44" s="1" t="n">
         <v>1.74</v>
       </c>
-      <c r="F44" s="0" t="n">
+      <c r="F44" s="1" t="n">
         <v>1.595</v>
       </c>
-      <c r="G44" s="0" t="n">
+      <c r="G44" s="1" t="n">
         <v>61.9574920222797</v>
       </c>
-      <c r="H44" s="0" t="n">
+      <c r="H44" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I44" s="0" t="s">
+      <c r="I44" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="J44" s="0" t="s">
+      <c r="J44" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="C45" s="1" t="n">
         <v>63.16</v>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="D45" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="E45" s="0" t="n">
+      <c r="E45" s="1" t="n">
         <v>1.65</v>
       </c>
-      <c r="F45" s="0" t="n">
+      <c r="F45" s="1" t="n">
         <v>1.515</v>
       </c>
-      <c r="G45" s="0" t="n">
+      <c r="G45" s="1" t="n">
         <v>62.769430941066</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="H45" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I45" s="0" t="s">
+      <c r="I45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J45" s="0" t="s">
+      <c r="J45" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="C46" s="1" t="n">
         <v>61.9</v>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="D46" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="1" t="n">
         <v>1.69</v>
       </c>
-      <c r="F46" s="0" t="n">
+      <c r="F46" s="1" t="n">
         <v>1.546</v>
       </c>
-      <c r="G46" s="0" t="n">
+      <c r="G46" s="1" t="n">
         <v>62.3980145503499</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="H46" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I46" s="0" t="s">
+      <c r="I46" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J46" s="0" t="s">
+      <c r="J46" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="C47" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="D47" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="E47" s="0" t="n">
+      <c r="E47" s="1" t="n">
         <v>1.68</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="F47" s="1" t="n">
         <v>1.543</v>
       </c>
-      <c r="G47" s="0" t="n">
+      <c r="G47" s="1" t="n">
         <v>63.3574920222797</v>
       </c>
-      <c r="H47" s="0" t="n">
+      <c r="H47" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I47" s="0" t="s">
+      <c r="I47" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J47" s="0" t="s">
+      <c r="J47" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="C48" s="1" t="n">
         <v>65.12</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="D48" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="E48" s="0" t="n">
+      <c r="E48" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="F48" s="1" t="n">
         <v>1.469</v>
       </c>
-      <c r="G48" s="0" t="n">
+      <c r="G48" s="1" t="n">
         <v>64.7720572274233</v>
       </c>
-      <c r="H48" s="0" t="n">
+      <c r="H48" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I48" s="0" t="s">
+      <c r="I48" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="J48" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C49" s="0" t="n">
+      <c r="C49" s="1" t="n">
         <v>68</v>
       </c>
-      <c r="D49" s="0" t="n">
+      <c r="D49" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="E49" s="0" t="n">
+      <c r="E49" s="1" t="n">
         <v>1.54</v>
       </c>
-      <c r="F49" s="0" t="n">
+      <c r="F49" s="1" t="n">
         <v>1.407</v>
       </c>
-      <c r="G49" s="0" t="n">
+      <c r="G49" s="1" t="n">
         <v>64.0213473454472</v>
       </c>
-      <c r="H49" s="0" t="n">
+      <c r="H49" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I49" s="0" t="s">
+      <c r="I49" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="J49" s="0" t="s">
+      <c r="J49" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C50" s="0" t="n">
+      <c r="C50" s="1" t="n">
         <v>63.33</v>
       </c>
-      <c r="D50" s="0" t="n">
+      <c r="D50" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E50" s="0" t="n">
+      <c r="E50" s="1" t="n">
         <v>1.65</v>
       </c>
-      <c r="F50" s="0" t="n">
+      <c r="F50" s="1" t="n">
         <v>1.511</v>
       </c>
-      <c r="G50" s="0" t="n">
+      <c r="G50" s="1" t="n">
         <v>61.6824750594602</v>
       </c>
-      <c r="H50" s="0" t="n">
+      <c r="H50" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I50" s="0" t="s">
+      <c r="I50" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J50" s="0" t="s">
+      <c r="J50" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="0" t="n">
+      <c r="C51" s="1" t="n">
         <v>60.98</v>
       </c>
-      <c r="D51" s="0" t="n">
+      <c r="D51" s="1" t="n">
         <v>41</v>
       </c>
-      <c r="E51" s="0" t="n">
+      <c r="E51" s="1" t="n">
         <v>1.71</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51" s="1" t="n">
         <v>1.569</v>
       </c>
-      <c r="G51" s="0" t="n">
+      <c r="G51" s="1" t="n">
         <v>61.6310790019832</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="H51" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I51" s="0" t="s">
+      <c r="I51" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J51" s="0" t="s">
+      <c r="J51" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="0" t="n">
+      <c r="C52" s="1" t="n">
         <v>65.79</v>
       </c>
-      <c r="D52" s="0" t="n">
+      <c r="D52" s="1" t="n">
         <v>38</v>
       </c>
-      <c r="E52" s="0" t="n">
+      <c r="E52" s="1" t="n">
         <v>1.59</v>
       </c>
-      <c r="F52" s="0" t="n">
+      <c r="F52" s="1" t="n">
         <v>1.455</v>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="G52" s="1" t="n">
         <v>64.610430941066</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="H52" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I52" s="0" t="s">
+      <c r="I52" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J52" s="0" t="s">
+      <c r="J52" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="0" t="n">
+      <c r="C53" s="1" t="n">
         <v>61.64</v>
       </c>
-      <c r="D53" s="0" t="n">
+      <c r="D53" s="1" t="n">
         <v>73</v>
       </c>
-      <c r="E53" s="0" t="n">
+      <c r="E53" s="1" t="n">
         <v>1.69</v>
       </c>
-      <c r="F53" s="0" t="n">
+      <c r="F53" s="1" t="n">
         <v>1.552</v>
       </c>
-      <c r="G53" s="0" t="n">
+      <c r="G53" s="1" t="n">
         <v>65.0361151644102</v>
       </c>
-      <c r="H53" s="0" t="n">
+      <c r="H53" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I53" s="0" t="s">
+      <c r="I53" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J53" s="0" t="s">
+      <c r="J53" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="0" t="n">
+      <c r="C54" s="1" t="n">
         <v>64.52</v>
       </c>
-      <c r="D54" s="0" t="n">
+      <c r="D54" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="E54" s="0" t="n">
+      <c r="E54" s="1" t="n">
         <v>1.62</v>
       </c>
-      <c r="F54" s="0" t="n">
+      <c r="F54" s="1" t="n">
         <v>1.483</v>
       </c>
-      <c r="G54" s="0" t="n">
+      <c r="G54" s="1" t="n">
         <v>62.6827549109574</v>
       </c>
-      <c r="H54" s="0" t="n">
+      <c r="H54" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I54" s="0" t="s">
+      <c r="I54" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J54" s="0" t="s">
+      <c r="J54" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C55" s="0" t="n">
+      <c r="C55" s="1" t="n">
         <v>73.08</v>
       </c>
-      <c r="D55" s="0" t="n">
+      <c r="D55" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E55" s="0" t="n">
+      <c r="E55" s="1" t="n">
         <v>1.43</v>
       </c>
-      <c r="F55" s="0" t="n">
+      <c r="F55" s="1" t="n">
         <v>1.309</v>
       </c>
-      <c r="G55" s="0" t="n">
+      <c r="G55" s="1" t="n">
         <v>67.7774348880764</v>
       </c>
-      <c r="H55" s="0" t="n">
+      <c r="H55" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I55" s="0" t="s">
+      <c r="I55" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J55" s="0" t="s">
+      <c r="J55" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C56" s="0" t="n">
+      <c r="C56" s="1" t="n">
         <v>65.38</v>
       </c>
-      <c r="D56" s="0" t="n">
+      <c r="D56" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E56" s="0" t="n">
+      <c r="E56" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="F56" s="0" t="n">
+      <c r="F56" s="1" t="n">
         <v>1.464</v>
       </c>
-      <c r="G56" s="0" t="n">
+      <c r="G56" s="1" t="n">
         <v>62.3874348880764</v>
       </c>
-      <c r="H56" s="0" t="n">
+      <c r="H56" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I56" s="0" t="s">
+      <c r="I56" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J56" s="0" t="s">
+      <c r="J56" s="1" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="0" t="n">
+      <c r="C57" s="1" t="n">
         <v>60.45</v>
       </c>
-      <c r="D57" s="0" t="n">
+      <c r="D57" s="1" t="n">
         <v>177</v>
       </c>
-      <c r="E57" s="0" t="n">
+      <c r="E57" s="1" t="n">
         <v>1.73</v>
       </c>
-      <c r="F57" s="0" t="n">
+      <c r="F57" s="1" t="n">
         <v>1.583</v>
       </c>
-      <c r="G57" s="0" t="n">
+      <c r="G57" s="1" t="n">
         <v>68.7215336146103</v>
       </c>
-      <c r="H57" s="0" t="n">
+      <c r="H57" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I57" s="0" t="s">
+      <c r="I57" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J57" s="0" t="s">
+      <c r="J57" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="0" t="n">
+      <c r="C58" s="1" t="n">
         <v>65.63</v>
       </c>
-      <c r="D58" s="0" t="n">
+      <c r="D58" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="E58" s="0" t="n">
+      <c r="E58" s="1" t="n">
         <v>1.59</v>
       </c>
-      <c r="F58" s="0" t="n">
+      <c r="F58" s="1" t="n">
         <v>1.458</v>
       </c>
-      <c r="G58" s="0" t="n">
+      <c r="G58" s="1" t="n">
         <v>63.6217233841622</v>
       </c>
-      <c r="H58" s="0" t="n">
+      <c r="H58" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I58" s="0" t="s">
+      <c r="I58" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J58" s="0" t="s">
+      <c r="J58" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C59" s="0" t="n">
+      <c r="C59" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D59" s="0" t="n">
+      <c r="D59" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="E59" s="0" t="n">
+      <c r="E59" s="1" t="n">
         <v>1.74</v>
       </c>
-      <c r="F59" s="0" t="n">
+      <c r="F59" s="1" t="n">
         <v>1.595</v>
       </c>
-      <c r="G59" s="0" t="n">
+      <c r="G59" s="1" t="n">
         <v>62.4437243758337</v>
       </c>
-      <c r="H59" s="0" t="n">
+      <c r="H59" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I59" s="0" t="s">
+      <c r="I59" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J59" s="0" t="s">
+      <c r="J59" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="0" t="n">
+      <c r="C60" s="1" t="n">
         <v>64.15</v>
       </c>
-      <c r="D60" s="0" t="n">
+      <c r="D60" s="1" t="n">
         <v>106</v>
       </c>
-      <c r="E60" s="0" t="n">
+      <c r="E60" s="1" t="n">
         <v>1.63</v>
       </c>
-      <c r="F60" s="0" t="n">
+      <c r="F60" s="1" t="n">
         <v>1.492</v>
       </c>
-      <c r="G60" s="0" t="n">
+      <c r="G60" s="1" t="n">
         <v>68.6959001015557</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="H60" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I60" s="0" t="s">
+      <c r="I60" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J60" s="0" t="s">
+      <c r="J60" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="0" t="n">
+      <c r="C61" s="1" t="n">
         <v>65.22</v>
       </c>
-      <c r="D61" s="0" t="n">
+      <c r="D61" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="E61" s="0" t="n">
+      <c r="E61" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="F61" s="0" t="n">
+      <c r="F61" s="1" t="n">
         <v>1.467</v>
       </c>
-      <c r="G61" s="0" t="n">
+      <c r="G61" s="1" t="n">
         <v>61.6499695312327</v>
       </c>
-      <c r="H61" s="0" t="n">
+      <c r="H61" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I61" s="0" t="s">
+      <c r="I61" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="J61" s="0" t="s">
+      <c r="J61" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="0" t="n">
+      <c r="C62" s="1" t="n">
         <v>63.39</v>
       </c>
-      <c r="D62" s="0" t="n">
+      <c r="D62" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="E62" s="0" t="n">
+      <c r="E62" s="1" t="n">
         <v>1.65</v>
       </c>
-      <c r="F62" s="0" t="n">
+      <c r="F62" s="1" t="n">
         <v>1.51</v>
       </c>
-      <c r="G62" s="0" t="n">
+      <c r="G62" s="1" t="n">
         <v>68.4447918709431</v>
       </c>
-      <c r="H62" s="0" t="n">
+      <c r="H62" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I62" s="0" t="s">
+      <c r="I62" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J62" s="0" t="s">
+      <c r="J62" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C63" s="0" t="n">
+      <c r="C63" s="1" t="n">
         <v>61.54</v>
       </c>
-      <c r="D63" s="0" t="n">
+      <c r="D63" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E63" s="0" t="n">
+      <c r="E63" s="1" t="n">
         <v>1.7</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="F63" s="1" t="n">
         <v>1.555</v>
       </c>
-      <c r="G63" s="0" t="n">
+      <c r="G63" s="1" t="n">
         <v>59.6994348880764</v>
       </c>
-      <c r="H63" s="0" t="n">
+      <c r="H63" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I63" s="0" t="s">
+      <c r="I63" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J63" s="0" t="s">
+      <c r="J63" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C64" s="0" t="n">
+      <c r="C64" s="1" t="n">
         <v>71.43</v>
       </c>
-      <c r="D64" s="0" t="n">
+      <c r="D64" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E64" s="0" t="n">
+      <c r="E64" s="1" t="n">
         <v>1.46</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="F64" s="1" t="n">
         <v>1.34</v>
       </c>
-      <c r="G64" s="0" t="n">
+      <c r="G64" s="1" t="n">
         <v>67.0005025172782</v>
       </c>
-      <c r="H64" s="0" t="n">
+      <c r="H64" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I64" s="0" t="s">
+      <c r="I64" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J64" s="0" t="s">
+      <c r="J64" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C65" s="0" t="n">
+      <c r="C65" s="1" t="n">
         <v>65.52</v>
       </c>
-      <c r="D65" s="0" t="n">
+      <c r="D65" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="E65" s="0" t="n">
+      <c r="E65" s="1" t="n">
         <v>1.59</v>
       </c>
-      <c r="F65" s="0" t="n">
+      <c r="F65" s="1" t="n">
         <v>1.461</v>
       </c>
-      <c r="G65" s="0" t="n">
+      <c r="G65" s="1" t="n">
         <v>63.0425236360735</v>
       </c>
-      <c r="H65" s="0" t="n">
+      <c r="H65" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I65" s="0" t="s">
+      <c r="I65" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J65" s="0" t="s">
+      <c r="J65" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="0" t="n">
+      <c r="C66" s="1" t="n">
         <v>68.89</v>
       </c>
-      <c r="D66" s="0" t="n">
+      <c r="D66" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="E66" s="0" t="n">
+      <c r="E66" s="1" t="n">
         <v>1.52</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F66" s="1" t="n">
         <v>1.389</v>
       </c>
-      <c r="G66" s="0" t="n">
+      <c r="G66" s="1" t="n">
         <v>74.7152764461967</v>
       </c>
-      <c r="H66" s="0" t="n">
+      <c r="H66" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I66" s="0" t="s">
+      <c r="I66" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J66" s="0" t="s">
+      <c r="J66" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C67" s="0" t="n">
+      <c r="C67" s="1" t="n">
         <v>63.83</v>
       </c>
-      <c r="D67" s="0" t="n">
+      <c r="D67" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="E67" s="0" t="n">
+      <c r="E67" s="1" t="n">
         <v>1.64</v>
       </c>
-      <c r="F67" s="0" t="n">
+      <c r="F67" s="1" t="n">
         <v>1.499</v>
       </c>
-      <c r="G67" s="0" t="n">
+      <c r="G67" s="1" t="n">
         <v>64.3228297998526</v>
       </c>
-      <c r="H67" s="0" t="n">
+      <c r="H67" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I67" s="0" t="s">
+      <c r="I67" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J67" s="0" t="s">
+      <c r="J67" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C68" s="0" t="n">
+      <c r="C68" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="D68" s="0" t="n">
+      <c r="D68" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E68" s="0" t="n">
+      <c r="E68" s="1" t="n">
         <v>1.39</v>
       </c>
-      <c r="F68" s="0" t="n">
+      <c r="F68" s="1" t="n">
         <v>1.276</v>
       </c>
-      <c r="G68" s="0" t="n">
+      <c r="G68" s="1" t="n">
         <v>69.4995025172782</v>
       </c>
-      <c r="H68" s="0" t="n">
+      <c r="H68" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I68" s="0" t="s">
+      <c r="I68" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J68" s="0" t="s">
+      <c r="J68" s="1" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+      <c r="A69" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C69" s="0" t="n">
+      <c r="C69" s="1" t="n">
         <v>62.16</v>
       </c>
-      <c r="D69" s="0" t="n">
+      <c r="D69" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="E69" s="0" t="n">
+      <c r="E69" s="1" t="n">
         <v>1.68</v>
       </c>
-      <c r="F69" s="0" t="n">
+      <c r="F69" s="1" t="n">
         <v>1.539</v>
       </c>
-      <c r="G69" s="0" t="n">
+      <c r="G69" s="1" t="n">
         <v>65.469525464908</v>
       </c>
-      <c r="H69" s="0" t="n">
+      <c r="H69" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I69" s="0" t="s">
+      <c r="I69" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J69" s="3" t="s">
+      <c r="J69" s="4" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+      <c r="A70" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C70" s="0" t="n">
+      <c r="C70" s="1" t="n">
         <v>63.86</v>
       </c>
-      <c r="D70" s="0" t="n">
+      <c r="D70" s="1" t="n">
         <v>83</v>
       </c>
-      <c r="E70" s="0" t="n">
+      <c r="E70" s="1" t="n">
         <v>1.64</v>
       </c>
-      <c r="F70" s="0" t="n">
+      <c r="F70" s="1" t="n">
         <v>1.498</v>
       </c>
-      <c r="G70" s="0" t="n">
+      <c r="G70" s="1" t="n">
         <v>67.2450617497543</v>
       </c>
-      <c r="H70" s="0" t="n">
+      <c r="H70" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I70" s="0" t="s">
+      <c r="I70" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J70" s="0" t="s">
+      <c r="J70" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+      <c r="A71" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C71" s="0" t="n">
+      <c r="C71" s="1" t="n">
         <v>66.67</v>
       </c>
-      <c r="D71" s="0" t="n">
+      <c r="D71" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="E71" s="0" t="n">
+      <c r="E71" s="1" t="n">
         <v>1.57</v>
       </c>
-      <c r="F71" s="0" t="n">
+      <c r="F71" s="1" t="n">
         <v>1.435</v>
       </c>
-      <c r="G71" s="0" t="n">
+      <c r="G71" s="1" t="n">
         <v>64.0204750594602</v>
       </c>
-      <c r="H71" s="0" t="n">
+      <c r="H71" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I71" s="0" t="s">
+      <c r="I71" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J71" s="0" t="s">
+      <c r="J71" s="1" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+      <c r="A72" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C72" s="0" t="n">
+      <c r="C72" s="1" t="n">
         <v>64.76</v>
       </c>
-      <c r="D72" s="0" t="n">
+      <c r="D72" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="E72" s="0" t="n">
+      <c r="E72" s="1" t="n">
         <v>1.61</v>
       </c>
-      <c r="F72" s="0" t="n">
+      <c r="F72" s="1" t="n">
         <v>1.478</v>
       </c>
-      <c r="G72" s="0" t="n">
+      <c r="G72" s="1" t="n">
         <v>69.0745435462411</v>
       </c>
-      <c r="H72" s="0" t="n">
+      <c r="H72" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I72" s="0" t="s">
+      <c r="I72" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="J72" s="4" t="s">
+      <c r="J72" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+      <c r="A73" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C73" s="0" t="n">
+      <c r="C73" s="1" t="n">
         <v>68.57</v>
       </c>
-      <c r="D73" s="0" t="n">
+      <c r="D73" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="E73" s="0" t="n">
+      <c r="E73" s="1" t="n">
         <v>1.52</v>
       </c>
-      <c r="F73" s="0" t="n">
+      <c r="F73" s="1" t="n">
         <v>1.396</v>
       </c>
-      <c r="G73" s="0" t="n">
+      <c r="G73" s="1" t="n">
         <v>66.1368868363369</v>
       </c>
-      <c r="H73" s="0" t="n">
+      <c r="H73" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I73" s="0" t="s">
+      <c r="I73" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="J73" s="0" t="s">
+      <c r="J73" s="1" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+      <c r="A74" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C74" s="0" t="n">
+      <c r="C74" s="1" t="n">
         <v>62.3</v>
       </c>
-      <c r="D74" s="0" t="n">
+      <c r="D74" s="1" t="n">
         <v>61</v>
       </c>
-      <c r="E74" s="0" t="n">
+      <c r="E74" s="1" t="n">
         <v>1.68</v>
       </c>
-      <c r="F74" s="0" t="n">
+      <c r="F74" s="1" t="n">
         <v>1.536</v>
       </c>
-      <c r="G74" s="0" t="n">
+      <c r="G74" s="1" t="n">
         <v>64.5819452659143</v>
       </c>
-      <c r="H74" s="0" t="n">
+      <c r="H74" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I74" s="0" t="s">
+      <c r="I74" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J74" s="0" t="s">
+      <c r="J74" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+      <c r="A75" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C75" s="0" t="n">
+      <c r="C75" s="1" t="n">
         <v>60.61</v>
       </c>
-      <c r="D75" s="0" t="n">
+      <c r="D75" s="1" t="n">
         <v>358</v>
       </c>
-      <c r="E75" s="0" t="n">
+      <c r="E75" s="1" t="n">
         <v>1.72</v>
       </c>
-      <c r="F75" s="0" t="n">
+      <c r="F75" s="1" t="n">
         <v>1.579</v>
       </c>
-      <c r="G75" s="0" t="n">
+      <c r="G75" s="1" t="n">
         <v>72.427</v>
       </c>
-      <c r="H75" s="0" t="n">
+      <c r="H75" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I75" s="0" t="s">
+      <c r="I75" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J75" s="0" t="s">
+      <c r="J75" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+      <c r="A76" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C76" s="0" t="n">
+      <c r="C76" s="1" t="n">
         <v>64.29</v>
       </c>
-      <c r="D76" s="0" t="n">
+      <c r="D76" s="1" t="n">
         <v>42</v>
       </c>
-      <c r="E76" s="0" t="n">
+      <c r="E76" s="1" t="n">
         <v>1.62</v>
       </c>
-      <c r="F76" s="0" t="n">
+      <c r="F76" s="1" t="n">
         <v>1.488</v>
       </c>
-      <c r="G76" s="0" t="n">
+      <c r="G76" s="1" t="n">
         <v>64.0710145503499</v>
       </c>
-      <c r="H76" s="0" t="n">
+      <c r="H76" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I76" s="0" t="s">
+      <c r="I76" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J76" s="0" t="s">
+      <c r="J76" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+      <c r="A77" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C77" s="0" t="n">
+      <c r="C77" s="1" t="n">
         <v>62.03</v>
       </c>
-      <c r="D77" s="0" t="n">
+      <c r="D77" s="1" t="n">
         <v>79</v>
       </c>
-      <c r="E77" s="0" t="n">
+      <c r="E77" s="1" t="n">
         <v>1.68</v>
       </c>
-      <c r="F77" s="0" t="n">
+      <c r="F77" s="1" t="n">
         <v>1.543</v>
       </c>
-      <c r="G77" s="0" t="n">
+      <c r="G77" s="1" t="n">
         <v>65.7120807365852</v>
       </c>
-      <c r="H77" s="0" t="n">
+      <c r="H77" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I77" s="0" t="s">
+      <c r="I77" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="J77" s="0" t="s">
+      <c r="J77" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+      <c r="A78" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C78" s="0" t="n">
+      <c r="C78" s="1" t="n">
         <v>60.71</v>
       </c>
-      <c r="D78" s="0" t="n">
+      <c r="D78" s="1" t="n">
         <v>28</v>
       </c>
-      <c r="E78" s="0" t="n">
+      <c r="E78" s="1" t="n">
         <v>1.72</v>
       </c>
-      <c r="F78" s="0" t="n">
+      <c r="F78" s="1" t="n">
         <v>1.576</v>
       </c>
-      <c r="G78" s="0" t="n">
+      <c r="G78" s="1" t="n">
         <v>59.4965025172782</v>
       </c>
-      <c r="H78" s="0" t="n">
+      <c r="H78" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I78" s="0" t="s">
+      <c r="I78" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="J78" s="0" t="s">
+      <c r="J78" s="1" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+      <c r="A79" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C79" s="0" t="n">
+      <c r="C79" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D79" s="0" t="n">
+      <c r="D79" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="E79" s="0" t="n">
+      <c r="E79" s="1" t="n">
         <v>1.74</v>
       </c>
-      <c r="F79" s="0" t="n">
+      <c r="F79" s="1" t="n">
         <v>1.595</v>
       </c>
-      <c r="G79" s="0" t="n">
+      <c r="G79" s="1" t="n">
         <v>60.8191077032209</v>
       </c>
-      <c r="H79" s="0" t="n">
+      <c r="H79" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I79" s="0" t="s">
+      <c r="I79" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J79" s="0" t="s">
+      <c r="J79" s="1" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+      <c r="A80" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C80" s="0" t="n">
+      <c r="C80" s="1" t="n">
         <v>62.14</v>
       </c>
-      <c r="D80" s="0" t="n">
+      <c r="D80" s="1" t="n">
         <v>103</v>
       </c>
-      <c r="E80" s="0" t="n">
+      <c r="E80" s="1" t="n">
         <v>1.68</v>
       </c>
-      <c r="F80" s="0" t="n">
+      <c r="F80" s="1" t="n">
         <v>1.54</v>
       </c>
-      <c r="G80" s="0" t="n">
+      <c r="G80" s="1" t="n">
         <v>67.1424332458362</v>
       </c>
-      <c r="H80" s="0" t="n">
+      <c r="H80" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I80" s="0" t="s">
+      <c r="I80" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J80" s="4" t="s">
+      <c r="J80" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+      <c r="A81" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C81" s="0" t="n">
+      <c r="C81" s="1" t="n">
         <v>69.23</v>
       </c>
-      <c r="D81" s="0" t="n">
+      <c r="D81" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E81" s="0" t="n">
+      <c r="E81" s="1" t="n">
         <v>1.51</v>
       </c>
-      <c r="F81" s="0" t="n">
+      <c r="F81" s="1" t="n">
         <v>1.382</v>
       </c>
-      <c r="G81" s="0" t="n">
+      <c r="G81" s="1" t="n">
         <v>65.0824348880764</v>
       </c>
-      <c r="H81" s="0" t="n">
+      <c r="H81" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I81" s="0" t="s">
+      <c r="I81" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="J81" s="3" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+      <c r="A82" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C82" s="0" t="n">
+      <c r="C82" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="D82" s="0" t="n">
+      <c r="D82" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="E82" s="0" t="n">
+      <c r="E82" s="1" t="n">
         <v>1.74</v>
       </c>
-      <c r="F82" s="0" t="n">
+      <c r="F82" s="1" t="n">
         <v>1.595</v>
       </c>
-      <c r="G82" s="0" t="n">
+      <c r="G82" s="1" t="n">
         <v>65.9798690526661</v>
       </c>
-      <c r="H82" s="0" t="n">
+      <c r="H82" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I82" s="0" t="s">
+      <c r="I82" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J82" s="0" t="s">
+      <c r="J82" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+      <c r="A83" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C83" s="0" t="n">
+      <c r="C83" s="1" t="n">
         <v>76.92</v>
       </c>
-      <c r="D83" s="0" t="n">
+      <c r="D83" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="E83" s="0" t="n">
+      <c r="E83" s="1" t="n">
         <v>1.36</v>
       </c>
-      <c r="F83" s="0" t="n">
+      <c r="F83" s="1" t="n">
         <v>1.244</v>
       </c>
-      <c r="G83" s="0" t="n">
+      <c r="G83" s="1" t="n">
         <v>70.4654348880764</v>
       </c>
-      <c r="H83" s="0" t="n">
+      <c r="H83" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I83" s="0" t="s">
+      <c r="I83" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J83" s="0" t="s">
+      <c r="J83" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+      <c r="A84" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C84" s="0" t="n">
+      <c r="C84" s="1" t="n">
         <v>63.64</v>
       </c>
-      <c r="D84" s="0" t="n">
+      <c r="D84" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="E84" s="0" t="n">
+      <c r="E84" s="1" t="n">
         <v>1.64</v>
       </c>
-      <c r="F84" s="0" t="n">
+      <c r="F84" s="1" t="n">
         <v>1.504</v>
       </c>
-      <c r="G84" s="0" t="n">
+      <c r="G84" s="1" t="n">
         <v>60.3171953799425</v>
       </c>
-      <c r="H84" s="0" t="n">
+      <c r="H84" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I84" s="0" t="s">
+      <c r="I84" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="J84" s="0" t="s">
+      <c r="J84" s="1" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
+      <c r="A85" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B85" s="0" t="s">
+      <c r="B85" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C85" s="0" t="n">
+      <c r="C85" s="1" t="n">
         <v>61.43</v>
       </c>
-      <c r="D85" s="0" t="n">
+      <c r="D85" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="E85" s="0" t="n">
+      <c r="E85" s="1" t="n">
         <v>1.7</v>
       </c>
-      <c r="F85" s="0" t="n">
+      <c r="F85" s="1" t="n">
         <v>1.558</v>
       </c>
-      <c r="G85" s="0" t="n">
+      <c r="G85" s="1" t="n">
         <v>64.6750315131694</v>
       </c>
-      <c r="H85" s="0" t="n">
+      <c r="H85" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I85" s="0" t="s">
+      <c r="I85" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="J85" s="0" t="s">
+      <c r="J85" s="1" t="s">
         <v>151</v>
       </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="J86" s="7"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>